<commit_message>
[ST - 15 April 2018 ] - Updated code for visualize tab, add input parameters and connection page validations for advance type ds
</commit_message>
<xml_diff>
--- a/TestData/ActualDataFile.xlsx
+++ b/TestData/ActualDataFile.xlsx
@@ -2,29 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_Local\Mosaic_RegressionSuite_UIPath\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -94,7 +90,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -106,7 +102,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -123,9 +119,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -153,31 +149,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -205,23 +184,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,9 +338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>